<commit_message>
actualizacion de la planificacion
</commit_message>
<xml_diff>
--- a/Documents/Scrum Documents.xlsx
+++ b/Documents/Scrum Documents.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="115">
   <si>
     <t xml:space="preserve">SPRINT 1
  </t>
@@ -320,21 +320,80 @@
     <t>Añadido de HTML y CSS a la pagina principal(Faltante)</t>
   </si>
   <si>
-    <t>Se debe reprogramar</t>
+    <t>Juan - Julian</t>
+  </si>
+  <si>
+    <t>Correccion de carrousel</t>
+  </si>
+  <si>
+    <t>Services y modularizacion de llamadas a la API</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>Peliculas destacadas e Item Pelicula component</t>
+  </si>
+  <si>
+    <t>2 dias</t>
+  </si>
+  <si>
+    <t>Julian - Andres</t>
+  </si>
+  <si>
+    <t>20/09/2017</t>
+  </si>
+  <si>
+    <t>27/09/2017</t>
+  </si>
+  <si>
+    <t>13/09/2017</t>
+  </si>
+  <si>
+    <t>Conexiones a la API / Bind de datos</t>
+  </si>
+  <si>
+    <t>Retoques al Header y Footer</t>
+  </si>
+  <si>
+    <t>Cambios en el routeo</t>
+  </si>
+  <si>
+    <t>Barra de busqueda</t>
+  </si>
+  <si>
+    <t>502 - 503</t>
+  </si>
+  <si>
+    <t>comienzo Pagina Pelicula component</t>
+  </si>
+  <si>
+    <t>Juan - Julian - Andres</t>
+  </si>
+  <si>
+    <t>Boton mas info de pelicula</t>
+  </si>
+  <si>
+    <t>User Score</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Inicio de implementacion de Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.34998626667073579"/>
@@ -386,21 +445,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="28"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
@@ -420,7 +464,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +509,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
@@ -807,15 +857,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
@@ -824,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -892,13 +942,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -916,19 +966,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -937,7 +978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
@@ -946,34 +987,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -982,31 +1023,31 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1039,6 +1080,12 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1097,6 +1144,106 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -1529,7 +1676,7 @@
   <dimension ref="B1:M53"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1574,47 +1721,47 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="78"/>
+      <c r="D4" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
@@ -1638,770 +1785,770 @@
       <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
     </row>
     <row r="7" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="49">
+      <c r="B7" s="46">
         <v>1</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="63">
         <v>42963</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="49">
         <v>1</v>
       </c>
-      <c r="H7" s="57" t="s">
+      <c r="H7" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
     </row>
     <row r="8" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="50">
+      <c r="B8" s="47">
         <v>2</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="64">
         <v>42963</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="52">
         <v>1</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
     </row>
     <row r="9" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="51">
+      <c r="B9" s="48">
         <v>3</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="65">
         <v>42970</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="51">
         <v>2</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
     </row>
     <row r="10" spans="2:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="50">
+      <c r="B10" s="47">
         <v>4</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="66">
         <v>42970</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="50">
         <v>2</v>
       </c>
-      <c r="H10" s="61" t="s">
+      <c r="H10" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
     </row>
     <row r="11" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="51">
+      <c r="B11" s="48">
         <v>5</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="65">
         <v>42977</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="51">
         <v>3</v>
       </c>
-      <c r="H11" s="60" t="s">
+      <c r="H11" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="47">
+        <v>6</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="66">
+        <v>42977</v>
+      </c>
+      <c r="F12" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="50">
+        <v>3</v>
+      </c>
+      <c r="H12" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-    </row>
-    <row r="12" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="50">
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+    </row>
+    <row r="13" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="48">
+        <v>7</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="65">
+        <v>42984</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="51">
+        <v>4</v>
+      </c>
+      <c r="H13" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+    </row>
+    <row r="14" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="47">
+        <v>8</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="66">
+        <v>42991</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="50">
+        <v>5</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" spans="2:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="48">
+        <v>9</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="65">
+        <v>42998</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="51">
         <v>6</v>
       </c>
-      <c r="C12" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="69">
-        <v>42977</v>
-      </c>
-      <c r="F12" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="53">
-        <v>3</v>
-      </c>
-      <c r="H12" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-    </row>
-    <row r="13" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="51">
-        <v>7</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="68">
-        <v>42984</v>
-      </c>
-      <c r="F13" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="54">
-        <v>4</v>
-      </c>
-      <c r="H13" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-    </row>
-    <row r="14" spans="2:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50">
-        <v>8</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="69">
-        <v>42991</v>
-      </c>
-      <c r="F14" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="53">
-        <v>5</v>
-      </c>
-      <c r="H14" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-    </row>
-    <row r="15" spans="2:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="51">
+      <c r="H15" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+    </row>
+    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="80"/>
+      <c r="D17" s="72">
         <v>9</v>
       </c>
-      <c r="C15" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="68">
-        <v>42998</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="54">
+      <c r="E17" s="50"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="80"/>
+      <c r="D18" s="72">
+        <v>0</v>
+      </c>
+      <c r="E18" s="50"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="29"/>
+    </row>
+    <row r="19" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="80"/>
+      <c r="D19" s="72">
         <v>6</v>
       </c>
-      <c r="H15" s="60" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-    </row>
-    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="29"/>
-    </row>
-    <row r="17" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="75">
-        <v>3</v>
-      </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="29"/>
-    </row>
-    <row r="18" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="81" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="75">
-        <v>6</v>
-      </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="29"/>
-    </row>
-    <row r="19" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="75">
-        <v>3</v>
-      </c>
-      <c r="E19" s="53"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="29"/>
     </row>
     <row r="20" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
       <c r="L20" s="29"/>
     </row>
     <row r="21" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="11"/>
     </row>
     <row r="22" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
       <c r="L22" s="11"/>
     </row>
     <row r="23" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
       <c r="L23" s="11"/>
     </row>
     <row r="24" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
       <c r="L24" s="11"/>
     </row>
     <row r="25" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
       <c r="L27" s="29"/>
     </row>
     <row r="28" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
       <c r="M28" s="37"/>
     </row>
     <row r="29" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
       <c r="M29" s="37"/>
     </row>
     <row r="30" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
       <c r="M30" s="37"/>
     </row>
     <row r="31" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
       <c r="M31" s="37"/>
     </row>
     <row r="32" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
       <c r="M32" s="37"/>
     </row>
     <row r="33" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
       <c r="M33" s="37"/>
     </row>
     <row r="34" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
       <c r="M34" s="37"/>
     </row>
     <row r="35" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
       <c r="M35" s="37"/>
     </row>
     <row r="36" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
       <c r="M36" s="37"/>
     </row>
     <row r="37" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
       <c r="M37" s="37"/>
     </row>
     <row r="38" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
       <c r="M38" s="37"/>
     </row>
     <row r="39" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
       <c r="L39" s="29"/>
       <c r="M39" s="37"/>
     </row>
     <row r="40" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
       <c r="M40" s="37"/>
     </row>
     <row r="41" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
       <c r="M41" s="37"/>
     </row>
     <row r="42" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
       <c r="M42" s="37"/>
     </row>
     <row r="43" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
       <c r="M43" s="37"/>
     </row>
     <row r="44" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
       <c r="M44" s="37"/>
     </row>
     <row r="45" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
       <c r="M45" s="37"/>
     </row>
     <row r="46" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
       <c r="M46" s="37"/>
     </row>
     <row r="47" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
       <c r="M47" s="37"/>
     </row>
     <row r="48" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
       <c r="M48" s="37"/>
     </row>
     <row r="49" spans="2:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
       <c r="M49" s="37"/>
     </row>
     <row r="50" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
       <c r="M50" s="37"/>
     </row>
     <row r="51" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
       <c r="L51" s="29"/>
       <c r="M51" s="37"/>
     </row>
     <row r="52" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="41"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="38"/>
       <c r="M52" s="37"/>
     </row>
     <row r="53" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2438,17 +2585,17 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L59"/>
+  <dimension ref="B1:L91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K91" sqref="K91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="45.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
@@ -2482,11 +2629,11 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="10" t="s">
         <v>90</v>
       </c>
@@ -2535,29 +2682,29 @@
       <c r="H7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="77" t="s">
+      <c r="I7" s="74" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="19">
         <v>9</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="73">
         <v>42956</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="78">
+      <c r="I8" s="75">
         <v>42963</v>
       </c>
     </row>
@@ -2596,7 +2743,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="89" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="33">
@@ -2625,7 +2772,7 @@
       </c>
     </row>
     <row r="12" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="91"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="35">
         <v>102</v>
       </c>
@@ -2652,7 +2799,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="91"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="35">
         <v>201</v>
       </c>
@@ -2679,17 +2826,17 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="92"/>
-      <c r="C14" s="85" t="s">
+      <c r="B14" s="91"/>
+      <c r="C14" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="87"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="86"/>
     </row>
     <row r="15" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
@@ -2731,24 +2878,24 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="19">
         <v>7</v>
       </c>
       <c r="F18" s="17">
         <v>2</v>
       </c>
-      <c r="G18" s="76">
+      <c r="G18" s="73">
         <v>42963</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="78">
+      <c r="I18" s="75">
         <v>42970</v>
       </c>
       <c r="J18" s="2"/>
@@ -2794,7 +2941,7 @@
       <c r="K20" s="29"/>
     </row>
     <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="92" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="33">
@@ -2824,7 +2971,7 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="94"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="35">
         <v>302</v>
       </c>
@@ -2852,7 +2999,7 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="94"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="35">
         <v>303</v>
       </c>
@@ -2880,7 +3027,7 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="94"/>
+      <c r="B24" s="93"/>
       <c r="C24" s="35">
         <v>304</v>
       </c>
@@ -2908,7 +3055,7 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="94"/>
+      <c r="B25" s="93"/>
       <c r="C25" s="35">
         <v>305</v>
       </c>
@@ -2936,7 +3083,7 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="94"/>
+      <c r="B26" s="93"/>
       <c r="C26" s="35">
         <v>306</v>
       </c>
@@ -2964,7 +3111,7 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="94"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="35">
         <v>307</v>
       </c>
@@ -2992,7 +3139,7 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="94"/>
+      <c r="B28" s="93"/>
       <c r="C28" s="35">
         <v>401</v>
       </c>
@@ -3020,17 +3167,17 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="95"/>
-      <c r="C29" s="85" t="s">
+      <c r="B29" s="94"/>
+      <c r="C29" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="86"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="87"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="86"/>
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="2:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3074,24 +3221,24 @@
       <c r="L32" s="37"/>
     </row>
     <row r="33" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="88"/>
       <c r="E33" s="19">
         <v>6</v>
       </c>
       <c r="F33" s="17">
         <v>3</v>
       </c>
-      <c r="G33" s="76">
+      <c r="G33" s="73">
         <v>42970</v>
       </c>
       <c r="H33" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="78">
+      <c r="I33" s="75">
         <v>42977</v>
       </c>
       <c r="L33" s="37"/>
@@ -3133,7 +3280,7 @@
       <c r="L35" s="37"/>
     </row>
     <row r="36" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="96" t="s">
+      <c r="B36" s="95" t="s">
         <v>84</v>
       </c>
       <c r="C36" s="33">
@@ -3163,7 +3310,7 @@
       <c r="L36" s="37"/>
     </row>
     <row r="37" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="97"/>
+      <c r="B37" s="96"/>
       <c r="C37" s="35">
         <v>502</v>
       </c>
@@ -3191,7 +3338,7 @@
       <c r="L37" s="37"/>
     </row>
     <row r="38" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="97"/>
+      <c r="B38" s="96"/>
       <c r="C38" s="35">
         <v>601</v>
       </c>
@@ -3219,7 +3366,7 @@
       <c r="L38" s="37"/>
     </row>
     <row r="39" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="97"/>
+      <c r="B39" s="96"/>
       <c r="C39" s="35">
         <v>602</v>
       </c>
@@ -3247,7 +3394,7 @@
       <c r="L39" s="37"/>
     </row>
     <row r="40" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="97"/>
+      <c r="B40" s="96"/>
       <c r="C40" s="35">
         <v>603</v>
       </c>
@@ -3275,7 +3422,7 @@
       <c r="L40" s="37"/>
     </row>
     <row r="41" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="97"/>
+      <c r="B41" s="96"/>
       <c r="C41" s="35">
         <v>604</v>
       </c>
@@ -3303,7 +3450,7 @@
       <c r="L41" s="37"/>
     </row>
     <row r="42" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="97"/>
+      <c r="B42" s="96"/>
       <c r="C42" s="35">
         <v>605</v>
       </c>
@@ -3331,17 +3478,17 @@
       <c r="L42" s="37"/>
     </row>
     <row r="43" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="98"/>
-      <c r="C43" s="85" t="s">
+      <c r="B43" s="97"/>
+      <c r="C43" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86"/>
-      <c r="G43" s="86"/>
-      <c r="H43" s="86"/>
-      <c r="I43" s="86"/>
-      <c r="J43" s="87"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="86"/>
       <c r="L43" s="37"/>
     </row>
     <row r="44" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3389,24 +3536,24 @@
       <c r="L46" s="37"/>
     </row>
     <row r="47" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="88" t="s">
+      <c r="B47" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
+      <c r="C47" s="88"/>
+      <c r="D47" s="88"/>
       <c r="E47" s="19">
         <v>5</v>
       </c>
       <c r="F47" s="17">
         <v>4</v>
       </c>
-      <c r="G47" s="76">
+      <c r="G47" s="73">
         <v>42977</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="78">
+      <c r="I47" s="75">
         <v>42984</v>
       </c>
       <c r="L47" s="37"/>
@@ -3448,7 +3595,7 @@
       <c r="L49" s="37"/>
     </row>
     <row r="50" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="81" t="s">
         <v>85</v>
       </c>
       <c r="C50" s="33" t="s">
@@ -3478,7 +3625,7 @@
       <c r="L50" s="37"/>
     </row>
     <row r="51" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="83"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="35" t="s">
         <v>26</v>
       </c>
@@ -3506,7 +3653,7 @@
       <c r="L51" s="37"/>
     </row>
     <row r="52" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="83"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="35">
         <v>604</v>
       </c>
@@ -3534,11 +3681,13 @@
       <c r="L52" s="37"/>
     </row>
     <row r="53" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="83"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="35">
         <v>501</v>
       </c>
-      <c r="D53" s="13"/>
+      <c r="D53" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="E53" s="10" t="s">
         <v>75</v>
       </c>
@@ -3548,17 +3697,25 @@
       <c r="G53" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="36"/>
+      <c r="H53" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J53" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="L53" s="37"/>
     </row>
     <row r="54" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="83"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="35">
         <v>502</v>
       </c>
-      <c r="D54" s="13"/>
+      <c r="D54" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="E54" s="10" t="s">
         <v>76</v>
       </c>
@@ -3568,17 +3725,25 @@
       <c r="G54" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="36"/>
+      <c r="H54" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J54" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="L54" s="37"/>
     </row>
     <row r="55" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="83"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="35">
         <v>401</v>
       </c>
-      <c r="D55" s="13"/>
+      <c r="D55" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="E55" s="10" t="s">
         <v>93</v>
       </c>
@@ -3588,23 +3753,29 @@
       <c r="G55" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H55" s="23"/>
-      <c r="I55" s="23"/>
-      <c r="J55" s="36"/>
+      <c r="H55" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J55" s="36" t="s">
+        <v>94</v>
+      </c>
       <c r="L55" s="37"/>
     </row>
     <row r="56" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="84"/>
-      <c r="C56" s="85" t="s">
+      <c r="B56" s="83"/>
+      <c r="C56" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="86"/>
-      <c r="H56" s="86"/>
-      <c r="I56" s="86"/>
-      <c r="J56" s="87"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="86"/>
       <c r="L56" s="37"/>
     </row>
     <row r="57" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3621,33 +3792,687 @@
       <c r="L57" s="37"/>
     </row>
     <row r="58" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="41"/>
-      <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="41"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="38"/>
       <c r="L58" s="37"/>
     </row>
     <row r="59" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="F59" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I59" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="K59" s="37"/>
       <c r="L59" s="37"/>
     </row>
+    <row r="60" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="88"/>
+      <c r="D60" s="88"/>
+      <c r="E60" s="19">
+        <v>3</v>
+      </c>
+      <c r="F60" s="17">
+        <v>5</v>
+      </c>
+      <c r="G60" s="73">
+        <v>42984</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="75">
+        <v>42991</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="123" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="33">
+        <v>605</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I63" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J63" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="124"/>
+      <c r="C64" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J64" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="124"/>
+      <c r="C65" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F65" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J65" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="124"/>
+      <c r="C66" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H66" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I66" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J66" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="124"/>
+      <c r="C67" s="35">
+        <v>401</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H67" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J67" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="125"/>
+      <c r="C68" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="85"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="85"/>
+      <c r="H68" s="85"/>
+      <c r="I68" s="85"/>
+      <c r="J68" s="86"/>
+    </row>
+    <row r="69" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+    </row>
+    <row r="70" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="31"/>
+      <c r="K70" s="122"/>
+    </row>
+    <row r="71" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="F71" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="G71" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="H71" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I71" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="88"/>
+      <c r="D72" s="88"/>
+      <c r="E72" s="19">
+        <v>2</v>
+      </c>
+      <c r="F72" s="17">
+        <v>6</v>
+      </c>
+      <c r="G72" s="73">
+        <v>42991</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="75">
+        <v>42998</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="98"/>
+      <c r="C73" s="98"/>
+      <c r="D73" s="98"/>
+      <c r="E73" s="99"/>
+      <c r="F73" s="99"/>
+      <c r="G73" s="100"/>
+      <c r="H73" s="100"/>
+      <c r="I73" s="101"/>
+      <c r="J73" s="99"/>
+    </row>
+    <row r="74" spans="2:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="99"/>
+      <c r="C74" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" s="104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="126" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="106" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="F75" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" s="109" t="s">
+        <v>59</v>
+      </c>
+      <c r="H75" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="I75" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="J75" s="110" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="127"/>
+      <c r="C76" s="111">
+        <v>501</v>
+      </c>
+      <c r="D76" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E76" s="113" t="s">
+        <v>107</v>
+      </c>
+      <c r="F76" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="H76" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="I76" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="J76" s="116" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="127"/>
+      <c r="C77" s="111">
+        <v>701</v>
+      </c>
+      <c r="D77" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" s="113" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="G77" s="115" t="s">
+        <v>55</v>
+      </c>
+      <c r="H77" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="I77" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="J77" s="116" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="128"/>
+      <c r="C78" s="117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="118"/>
+      <c r="E78" s="118"/>
+      <c r="F78" s="118"/>
+      <c r="G78" s="118"/>
+      <c r="H78" s="118"/>
+      <c r="I78" s="118"/>
+      <c r="J78" s="119"/>
+    </row>
+    <row r="79" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="120"/>
+      <c r="C79" s="120"/>
+      <c r="D79" s="120"/>
+      <c r="E79" s="120"/>
+      <c r="F79" s="121"/>
+      <c r="G79" s="121"/>
+      <c r="H79" s="121"/>
+      <c r="I79" s="121"/>
+      <c r="J79" s="121"/>
+    </row>
+    <row r="80" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="30"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="30"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="32"/>
+      <c r="J80" s="31"/>
+      <c r="K80" s="31"/>
+    </row>
+    <row r="81" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="F81" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="G81" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I81" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="88"/>
+      <c r="D82" s="88"/>
+      <c r="E82" s="19">
+        <v>2</v>
+      </c>
+      <c r="F82" s="17">
+        <v>7</v>
+      </c>
+      <c r="G82" s="73">
+        <v>42998</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I82" s="75">
+        <v>43005</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="98"/>
+      <c r="C83" s="98"/>
+      <c r="D83" s="98"/>
+      <c r="E83" s="99"/>
+      <c r="F83" s="99"/>
+      <c r="G83" s="100"/>
+      <c r="H83" s="100"/>
+      <c r="I83" s="101"/>
+      <c r="J83" s="99"/>
+    </row>
+    <row r="84" spans="2:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="99"/>
+      <c r="C84" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="102" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="I84" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="J84" s="104" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="129" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" s="105">
+        <v>701</v>
+      </c>
+      <c r="D85" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="F85" s="108" t="s">
+        <v>97</v>
+      </c>
+      <c r="G85" s="109" t="s">
+        <v>59</v>
+      </c>
+      <c r="H85" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="I85" s="108" t="s">
+        <v>99</v>
+      </c>
+      <c r="J85" s="110" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="130"/>
+      <c r="C86" s="111">
+        <v>901</v>
+      </c>
+      <c r="D86" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="113" t="s">
+        <v>112</v>
+      </c>
+      <c r="F86" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="G86" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="H86" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="I86" s="114" t="s">
+        <v>99</v>
+      </c>
+      <c r="J86" s="116" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="130"/>
+      <c r="C87" s="111">
+        <v>801</v>
+      </c>
+      <c r="D87" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="113" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="G87" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="H87" s="114" t="s">
+        <v>26</v>
+      </c>
+      <c r="I87" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="J87" s="116" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="130"/>
+      <c r="C88" s="111" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="113" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="114" t="s">
+        <v>97</v>
+      </c>
+      <c r="G88" s="115" t="s">
+        <v>74</v>
+      </c>
+      <c r="H88" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="I88" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="J88" s="116" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="131"/>
+      <c r="C89" s="117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="118"/>
+      <c r="E89" s="118"/>
+      <c r="F89" s="118"/>
+      <c r="G89" s="118"/>
+      <c r="H89" s="118"/>
+      <c r="I89" s="118"/>
+      <c r="J89" s="119"/>
+    </row>
+    <row r="90" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="120"/>
+      <c r="C90" s="120"/>
+      <c r="D90" s="120"/>
+      <c r="E90" s="120"/>
+      <c r="F90" s="121"/>
+      <c r="G90" s="121"/>
+      <c r="H90" s="121"/>
+      <c r="I90" s="121"/>
+      <c r="J90" s="121"/>
+    </row>
+    <row r="91" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K91" s="31"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="22">
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C78:J78"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="C89:J89"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B63:B68"/>
+    <mergeCell ref="C68:J68"/>
     <mergeCell ref="B50:B56"/>
     <mergeCell ref="C56:J56"/>
     <mergeCell ref="B3:D3"/>
@@ -3662,9 +4487,12 @@
     <mergeCell ref="C43:J43"/>
     <mergeCell ref="C14:J14"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E64" r:id="rId1" tooltip="Agregado de services y modularizacion de llamadas a la api" display="https://github.com/julianpoma/tmbdttads/commit/ff2c80071a8701fa32124443751467a687ec951b" xr:uid="{736214EC-4317-43FF-892C-421CEDC53779}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <picture r:id="rId2"/>
+  <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId2"/>
+  <picture r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>